<commit_message>
Nomenclatura adecauda Encuesta Satisfaccion SYE
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Encuestas de Satisfaccion/SYE_EncuestaSatisfaccion-150427.xlsx
+++ b/qualtcom/Procesos/Encuestas de Satisfaccion/SYE_EncuestaSatisfaccion-150427.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>Encuesta de Satisfacción al Cliente</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>SYE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1447,7 @@
   <dimension ref="A1:AMK22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:F5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1522,6 +1525,9 @@
       <c r="D7" s="126"/>
       <c r="E7" s="126"/>
       <c r="F7" s="126"/>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="68" t="s">

</xml_diff>